<commit_message>
Added Template feature with Maven structure and latest Selenium jar files and web-drivers.
</commit_message>
<xml_diff>
--- a/Parcel-Test-Features/Custom-Template-Asthetic/src/test/java/Test_Data/Templates_Feature.xlsx
+++ b/Parcel-Test-Features/Custom-Template-Asthetic/src/test/java/Test_Data/Templates_Feature.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
@@ -10,6 +10,7 @@
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Template Information" sheetId="2" r:id="rId2"/>
     <sheet name="Template Setup" sheetId="3" r:id="rId3"/>
+    <sheet name="URL" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -72,13 +73,19 @@
   </si>
   <si>
     <t>001Template</t>
+  </si>
+  <si>
+    <t>Parcel URL</t>
+  </si>
+  <si>
+    <t>https://uat.parcelplatform.com/reporting/login.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +97,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,10 +127,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -131,8 +147,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,10 +525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,13 +582,40 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1567</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>